<commit_message>
ungoogled and update readme
</commit_message>
<xml_diff>
--- a/files/browser-benchmark-results.xlsx
+++ b/files/browser-benchmark-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\browser-benchmark-results\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ED702D-94E6-4762-84F4-5D940BDC7410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6186363-AA0B-4E2C-8469-E08B40F86952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="13176" windowHeight="23256" xr2:uid="{8B822904-8CBE-4657-805A-0AE50094A3AA}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{8B822904-8CBE-4657-805A-0AE50094A3AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,9 +705,21 @@
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B14" s="2">
+        <v>210</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1379</v>
+      </c>
+      <c r="D14" s="2">
+        <v>198</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1760</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>886.75</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>